<commit_message>
added warning messages for common errorss
</commit_message>
<xml_diff>
--- a/debug/output.xlsx
+++ b/debug/output.xlsx
@@ -390,13 +390,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK3"/>
+  <dimension ref="A1:BK2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
       <selection activeCell="BL1" sqref="BL1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="14.42578125" customWidth="1" min="5" max="5"/>
@@ -915,424 +915,142 @@
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
+          <t>Lumi#2340</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>N-ZAP '85</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t>463</t>
+        </is>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
           <t>AC Drift#2709</t>
         </is>
       </c>
-      <c r="AK2" t="inlineStr">
+      <c r="AR2" t="inlineStr">
         <is>
           <t>Dark Tetra Dualies</t>
         </is>
       </c>
-      <c r="AL2" t="inlineStr">
+      <c r="AS2" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="AM2" t="inlineStr">
+      <c r="AT2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AN2" t="inlineStr">
+      <c r="AU2" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="AO2" t="inlineStr">
+      <c r="AV2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AP2" t="inlineStr">
+      <c r="AW2" t="inlineStr">
         <is>
           <t>450</t>
         </is>
       </c>
-      <c r="AQ2" t="inlineStr">
+      <c r="AX2" t="inlineStr">
         <is>
           <t>ColeAurion#2631</t>
         </is>
       </c>
-      <c r="AR2" t="inlineStr">
+      <c r="AY2" t="inlineStr">
         <is>
           <t>Splattershot</t>
         </is>
       </c>
-      <c r="AS2" t="inlineStr">
+      <c r="AZ2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="AT2" t="inlineStr">
+      <c r="BA2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AU2" t="inlineStr">
+      <c r="BB2" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="AV2" t="inlineStr">
+      <c r="BC2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AW2" t="inlineStr">
+      <c r="BD2" t="inlineStr">
         <is>
           <t>298</t>
         </is>
       </c>
-      <c r="AX2" t="inlineStr">
+      <c r="BE2" t="inlineStr">
         <is>
           <t>Crummy#3603</t>
         </is>
       </c>
-      <c r="AY2" t="inlineStr">
+      <c r="BF2" t="inlineStr">
         <is>
           <t>Ballpoint Splatling</t>
         </is>
       </c>
-      <c r="AZ2" t="inlineStr">
+      <c r="BG2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="BA2" t="inlineStr">
+      <c r="BH2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="BB2" t="inlineStr">
+      <c r="BI2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="BC2" t="inlineStr">
+      <c r="BJ2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="BD2" t="inlineStr">
+      <c r="BK2" t="inlineStr">
         <is>
           <t>345</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Shipshape Cargo Co.</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Splat Zones</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>High Riders</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>LG Equinox</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Yoshi#1173</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Heavy Edit Splatling</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>1402</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Cash Flow#2279</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>Annaki Splattershot Nova</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>1441</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>fuyu#2908</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>.52 Gal</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>943</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>collin#1264</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>Dapple Dualies Nouveau</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>1044</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>IIIIXXIIII#2429</t>
-        </is>
-      </c>
-      <c r="AK3" t="inlineStr">
-        <is>
-          <t>Painbrush</t>
-        </is>
-      </c>
-      <c r="AL3" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="AM3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AN3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="AO3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AP3" t="inlineStr">
-        <is>
-          <t>1291</t>
-        </is>
-      </c>
-      <c r="AQ3" t="inlineStr">
-        <is>
-          <t>hambsa★#2687</t>
-        </is>
-      </c>
-      <c r="AR3" t="inlineStr">
-        <is>
-          <t>Dapple Dualies Nouveau</t>
-        </is>
-      </c>
-      <c r="AS3" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="AT3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="AU3" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="AV3" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="AW3" t="inlineStr">
-        <is>
-          <t>1243</t>
-        </is>
-      </c>
-      <c r="AX3" t="inlineStr">
-        <is>
-          <t>ClownNine#1886</t>
-        </is>
-      </c>
-      <c r="AY3" t="inlineStr">
-        <is>
-          <t>Hero Shot Replica</t>
-        </is>
-      </c>
-      <c r="AZ3" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="BA3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="BB3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="BC3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="BD3" t="inlineStr">
-        <is>
-          <t>1022</t>
-        </is>
-      </c>
-      <c r="BE3" t="inlineStr">
-        <is>
-          <t>MLG#1242</t>
-        </is>
-      </c>
-      <c r="BF3" t="inlineStr">
-        <is>
-          <t>Hydra Splatling</t>
-        </is>
-      </c>
-      <c r="BG3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="BH3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BI3" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="BJ3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="BK3" t="inlineStr">
-        <is>
-          <t>1007</t>
         </is>
       </c>
     </row>

</xml_diff>